<commit_message>
My Contact tests combined with Jonnies
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ContactPage - Kevins Copy.xlsx
+++ b/Testing Spreadsheet v1.0 ContactPage - Kevins Copy.xlsx
@@ -1094,7 +1094,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1104,7 +1103,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1114,7 +1112,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1179,7 +1176,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1276,11 +1272,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108871040"/>
-        <c:axId val="65148032"/>
+        <c:axId val="42246912"/>
+        <c:axId val="42248448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108871040"/>
+        <c:axId val="42246912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,7 +1285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65148032"/>
+        <c:crossAx val="42248448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1297,7 +1293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65148032"/>
+        <c:axId val="42248448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108871040"/>
+        <c:crossAx val="42246912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1737,13 +1733,13 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
@@ -1986,8 +1982,8 @@
   </sheetPr>
   <dimension ref="A1:Z163"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,7 +2536,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:26" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
@@ -2554,7 +2550,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
       <c r="G17" s="10"/>
@@ -2568,7 +2564,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
       <c r="G18" s="10"/>
@@ -2582,7 +2578,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
       <c r="G19" s="10"/>
@@ -2596,7 +2592,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
       <c r="G20" s="10"/>
@@ -2610,7 +2606,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
       <c r="G21" s="10"/>
@@ -2624,7 +2620,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
       <c r="G22" s="10"/>
@@ -2638,7 +2634,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
       <c r="G23" s="10"/>
@@ -2652,7 +2648,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="5:21" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
       <c r="G24" s="10"/>
@@ -4700,8 +4696,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5260,6 +5256,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5373,32 +5384,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -5413,9 +5402,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>